<commit_message>
updating covid vs flu comparison in Italy
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
+++ b/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy\Projects\COVID-19\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C93E00-8703-4C89-9B9D-116B6713FADA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365DB38E-7427-48D6-9B3A-EC2281AA525C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="112">
   <si>
     <t>https://www.cdc.gov/flu/weekly/#S2</t>
   </si>
@@ -355,15 +355,70 @@
   <si>
     <t>Rosano et. Al.</t>
   </si>
+  <si>
+    <t>% Hospitalized</t>
+  </si>
+  <si>
+    <t>Illnesses</t>
+  </si>
+  <si>
+    <t>Hospitalized</t>
+  </si>
+  <si>
+    <t>Deaths</t>
+  </si>
+  <si>
+    <t>Covid % hospitalized</t>
+  </si>
+  <si>
+    <t>Influenza burden, millions</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>https://www.nbcnewyork.com/news/local/as-nyc-nears-1000-covid-19-deaths-how-does-it-compare-to-typical-flu-seasons/2352180/</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov/flu/about/burden-averted/2017-2018.htm</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov/mmwr/volumes/69/wr/mm6912e2.htm#T1_down</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov/flu/about/burden/2017-2018.htm</t>
+  </si>
+  <si>
+    <t>COMPARE HOSPITALIZATION RATES BY AGE FOR FLU AND COVID</t>
+  </si>
+  <si>
+    <t>COMPARE DEATH COUNTS AND TIMING</t>
+  </si>
+  <si>
+    <t>https://www.vox.com/science-and-health/2020/4/2/21197617/coronavirus-pandemic-covid-19-death-rate-transmission-risk-factors-lockdowns-social-distancing</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/article/coronavirus-vs-flu.html</t>
+  </si>
+  <si>
+    <t>https://www.npr.org/sections/goatsandsoda/2020/03/20/815408287/how-the-novel-coronavirus-and-the-flu-are-alike-and-different</t>
+  </si>
+  <si>
+    <t>https://www.businessinsider.com/coronavirus-compared-seasonal-flu-in-the-us-death-rates-2020-3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,6 +453,14 @@
       <color rgb="FF2E2E2E"/>
       <name val="Georgia"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -525,12 +588,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -567,6 +631,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -585,19 +664,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
@@ -619,16 +688,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:colOff>60960</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>1802</xdr:rowOff>
+      <xdr:rowOff>24662</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -658,7 +727,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12283440" y="1135380"/>
+          <a:off x="11742420" y="1158240"/>
           <a:ext cx="2948940" cy="2524022"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -680,16 +749,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>331663</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>545023</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>7619</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>220979</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -719,7 +788,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8866063" y="1074420"/>
+          <a:off x="8469823" y="381000"/>
           <a:ext cx="2723956" cy="3078480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -752,8 +821,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>148046</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>542493</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>464820</xdr:rowOff>
     </xdr:to>
@@ -929,16 +998,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>62754</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>376518</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>236221</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>69029</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -968,8 +1037,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4267200" y="6766560"/>
-          <a:ext cx="9144000" cy="3276600"/>
+          <a:off x="2501154" y="6113930"/>
+          <a:ext cx="9147138" cy="3215640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1254,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:O44"/>
+  <dimension ref="D2:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1272,6 +1341,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="6" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
         <v>1</v>
@@ -1312,32 +1386,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D17" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D18" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D19" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D20" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D21" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D22" s="1" t="s">
         <v>81</v>
       </c>
@@ -1351,7 +1425,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D23" s="1" t="s">
         <v>82</v>
       </c>
@@ -1366,67 +1440,106 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D24" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D25" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D26" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="R26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D27" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="N27">
         <f>AVERAGE(61, 12)</f>
         <v>36.5</v>
       </c>
-      <c r="O27" s="20">
+      <c r="O27" s="15">
         <f>N27/N29</f>
         <v>1.3443830570902394E-3</v>
       </c>
-    </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="R27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="4:18" x14ac:dyDescent="0.3">
       <c r="N28">
         <f>AVERAGE(810, 140)</f>
         <v>475</v>
       </c>
-      <c r="O28" s="20">
+      <c r="O28" s="15">
         <f>N28/N29</f>
         <v>1.7495395948434623E-2</v>
       </c>
     </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:18" x14ac:dyDescent="0.3">
       <c r="N29">
         <f>AVERAGE(45000, 9300)</f>
         <v>27150</v>
       </c>
     </row>
+    <row r="30" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D30" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D31" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D32" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="38" spans="4:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="16" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D40" s="23"/>
+      <c r="D40" s="18"/>
     </row>
     <row r="41" spans="4:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="D41" s="21" t="s">
+      <c r="D41" s="16" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1436,7 +1549,7 @@
       </c>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D44" s="24" t="s">
+      <c r="D44" s="19" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1463,22 +1576,34 @@
     <hyperlink ref="D25" r:id="rId19" xr:uid="{DF793563-C909-4AFA-8D91-EF7BA935A96A}"/>
     <hyperlink ref="D26" r:id="rId20" xr:uid="{F1345CC6-6192-46FA-ABE2-FF04EFFFFC50}"/>
     <hyperlink ref="D39" r:id="rId21" display="https://www.cdc.gov/nndss/document/MMWR_Week_overview.pdf" xr:uid="{97D1A950-B2D5-4F55-84EE-6C6072B1BB4C}"/>
+    <hyperlink ref="D4" r:id="rId22" xr:uid="{C4235454-2F24-418F-8F59-96F1E822E69F}"/>
+    <hyperlink ref="D27" r:id="rId23" xr:uid="{659337CF-EAD8-45E5-B837-4315A2A254AE}"/>
+    <hyperlink ref="D30" r:id="rId24" location="T1_down" display="https://www.cdc.gov/mmwr/volumes/69/wr/mm6912e2.htm - T1_down" xr:uid="{3A613641-AEE8-475C-8548-B34EED9DE21B}"/>
+    <hyperlink ref="D31" r:id="rId25" xr:uid="{7A1072CB-A11B-491D-A0A2-78934EA3243D}"/>
+    <hyperlink ref="D32" r:id="rId26" xr:uid="{7097EADF-CDD3-40A3-8D24-A16CFE8A7DD9}"/>
+    <hyperlink ref="D33" r:id="rId27" xr:uid="{F524630E-8B26-4B47-9B8E-8BA0C6C1577B}"/>
+    <hyperlink ref="D34" r:id="rId28" xr:uid="{BC2124EB-8AF7-4071-B66B-C863476AD2EA}"/>
+    <hyperlink ref="D35" r:id="rId29" xr:uid="{0F82DACF-9546-4BFE-BA6C-391D28757EF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
-  <drawing r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
+  <drawing r:id="rId31"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F961DF-88C5-4FC4-A498-BDBE2D214606}">
-  <dimension ref="C3:P14"/>
+  <dimension ref="C3:Q44"/>
   <sheetViews>
-    <sheetView topLeftCell="H37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="20.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
@@ -1499,26 +1624,26 @@
       <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="18" t="s">
+      <c r="G4" s="28"/>
+      <c r="H4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="18" t="s">
+      <c r="I4" s="28"/>
+      <c r="J4" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="18" t="s">
+      <c r="K4" s="28"/>
+      <c r="L4" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="19"/>
-      <c r="N4" s="18" t="s">
+      <c r="M4" s="28"/>
+      <c r="N4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="19"/>
+      <c r="O4" s="28"/>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
@@ -1591,13 +1716,13 @@
       </c>
     </row>
     <row r="7" spans="3:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="12">
@@ -1636,11 +1761,11 @@
       </c>
     </row>
     <row r="8" spans="3:16" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="15"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="17"/>
+      <c r="E8" s="26"/>
       <c r="F8" s="13" t="s">
         <v>22</v>
       </c>
@@ -1674,13 +1799,13 @@
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="3:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="23" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="25" t="s">
         <v>34</v>
       </c>
       <c r="F9" s="12">
@@ -1719,11 +1844,11 @@
       </c>
     </row>
     <row r="10" spans="3:16" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="15"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="17"/>
+      <c r="E10" s="26"/>
       <c r="F10" s="13" t="s">
         <v>37</v>
       </c>
@@ -1757,13 +1882,13 @@
       <c r="P10" s="4"/>
     </row>
     <row r="11" spans="3:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="23" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="25" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="12">
@@ -1802,11 +1927,11 @@
       </c>
     </row>
     <row r="12" spans="3:16" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="15"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="13" t="s">
         <v>50</v>
       </c>
@@ -1840,13 +1965,13 @@
       <c r="P12" s="4"/>
     </row>
     <row r="13" spans="3:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="23" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="25" t="s">
         <v>61</v>
       </c>
       <c r="F13" s="12">
@@ -1885,11 +2010,11 @@
       </c>
     </row>
     <row r="14" spans="3:16" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="15"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="17"/>
+      <c r="E14" s="26"/>
       <c r="F14" s="13" t="s">
         <v>63</v>
       </c>
@@ -1921,23 +2046,219 @@
         <v>71</v>
       </c>
     </row>
+    <row r="35" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H35" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35">
+        <f t="shared" ref="I35:N35" si="0">J35-1</f>
+        <v>2010</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+      <c r="O35">
+        <v>2016</v>
+      </c>
+      <c r="P35">
+        <v>2017</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>97</v>
+      </c>
+      <c r="I36">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="J36">
+        <v>1.2E-2</v>
+      </c>
+      <c r="K36">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="L36">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="M36">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="N36">
+        <v>2.3E-2</v>
+      </c>
+      <c r="O36">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="P36">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="Q36">
+        <f>AVERAGE(I36:P36)</f>
+        <v>3.7874999999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H37" t="s">
+        <v>96</v>
+      </c>
+      <c r="I37">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J37">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K37">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L37">
+        <v>0.35</v>
+      </c>
+      <c r="M37">
+        <v>0.59</v>
+      </c>
+      <c r="N37">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="O37">
+        <v>0.497</v>
+      </c>
+      <c r="P37">
+        <v>0.81</v>
+      </c>
+      <c r="Q37" s="20">
+        <f>AVERAGE(I37:P37)</f>
+        <v>0.44087499999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>95</v>
+      </c>
+      <c r="I38">
+        <v>21</v>
+      </c>
+      <c r="J38">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="K38">
+        <v>34</v>
+      </c>
+      <c r="L38">
+        <v>30</v>
+      </c>
+      <c r="M38">
+        <v>30</v>
+      </c>
+      <c r="N38">
+        <v>24</v>
+      </c>
+      <c r="O38">
+        <v>29</v>
+      </c>
+      <c r="P38">
+        <v>45</v>
+      </c>
+      <c r="Q38" s="20">
+        <f>AVERAGE(I38:P38)</f>
+        <v>27.787500000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>94</v>
+      </c>
+      <c r="I40" s="14">
+        <f t="shared" ref="I40:Q40" si="1">I37/I38</f>
+        <v>1.3809523809523808E-2</v>
+      </c>
+      <c r="J40" s="14">
+        <f t="shared" si="1"/>
+        <v>1.5053763440860216E-2</v>
+      </c>
+      <c r="K40" s="14">
+        <f t="shared" si="1"/>
+        <v>1.6764705882352939E-2</v>
+      </c>
+      <c r="L40" s="14">
+        <f t="shared" si="1"/>
+        <v>1.1666666666666665E-2</v>
+      </c>
+      <c r="M40" s="14">
+        <f t="shared" si="1"/>
+        <v>1.9666666666666666E-2</v>
+      </c>
+      <c r="N40" s="14">
+        <f t="shared" si="1"/>
+        <v>1.1666666666666667E-2</v>
+      </c>
+      <c r="O40" s="14">
+        <f t="shared" si="1"/>
+        <v>1.7137931034482759E-2</v>
+      </c>
+      <c r="P40" s="14">
+        <f t="shared" si="1"/>
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="Q40" s="14">
+        <f t="shared" si="1"/>
+        <v>1.5865946918578497E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q42" s="14">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="44" spans="8:17" x14ac:dyDescent="0.3">
+      <c r="H44" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q44" s="22">
+        <f>Q42/Q40</f>
+        <v>11.975333144315282</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
going back some commits after accidentally adding sqlite; adding state-county economic data; updated US covid analyses; more comparisons to influenza
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
+++ b/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy\Projects\COVID-19\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365DB38E-7427-48D6-9B3A-EC2281AA525C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFE11F3-0652-438E-9CEB-B922DC577665}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="114">
   <si>
     <t>https://www.cdc.gov/flu/weekly/#S2</t>
   </si>
@@ -408,6 +408,12 @@
   </si>
   <si>
     <t>https://www.businessinsider.com/coronavirus-compared-seasonal-flu-in-the-us-death-rates-2020-3</t>
+  </si>
+  <si>
+    <t>https://www.bbc.com/future/article/20200401-coronavirus-why-death-and-mortality-rates-differ</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/2020/04/04/world/europe/germany-coronavirus-death-rate.html</t>
   </si>
 </sst>
 </file>
@@ -1325,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D2:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1366,6 +1372,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="11" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
     <row r="12" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D12" s="1" t="s">
         <v>73</v>
@@ -1485,6 +1496,9 @@
       </c>
     </row>
     <row r="29" spans="4:18" x14ac:dyDescent="0.3">
+      <c r="D29" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="N29">
         <f>AVERAGE(45000, 9300)</f>
         <v>27150</v>
@@ -1584,10 +1598,12 @@
     <hyperlink ref="D33" r:id="rId27" xr:uid="{F524630E-8B26-4B47-9B8E-8BA0C6C1577B}"/>
     <hyperlink ref="D34" r:id="rId28" xr:uid="{BC2124EB-8AF7-4071-B66B-C863476AD2EA}"/>
     <hyperlink ref="D35" r:id="rId29" xr:uid="{0F82DACF-9546-4BFE-BA6C-391D28757EF3}"/>
+    <hyperlink ref="D29" r:id="rId30" xr:uid="{C7889458-3269-414C-9333-27436CF7008C}"/>
+    <hyperlink ref="D11" r:id="rId31" xr:uid="{F68D2B68-E29A-4C59-AA25-381D80FDD725}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
-  <drawing r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
+  <drawing r:id="rId33"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
adding daily r0 tracking plots, updating other analyses
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
+++ b/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy\Projects\COVID-19\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFE11F3-0652-438E-9CEB-B922DC577665}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BB7576-74FE-4EC2-9565-008FD3DD90B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature" sheetId="1" r:id="rId1"/>
-    <sheet name="notes" sheetId="2" r:id="rId2"/>
+    <sheet name="data sources" sheetId="3" r:id="rId2"/>
+    <sheet name="notes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="151">
   <si>
     <t>https://www.cdc.gov/flu/weekly/#S2</t>
   </si>
@@ -415,6 +416,117 @@
   <si>
     <t>https://www.nytimes.com/2020/04/04/world/europe/germany-coronavirus-death-rate.html</t>
   </si>
+  <si>
+    <t>Lockdowns</t>
+  </si>
+  <si>
+    <t>https://auravision.ai/covid19-lockdown-tracker/</t>
+  </si>
+  <si>
+    <t>Death Rates</t>
+  </si>
+  <si>
+    <t>https://www.who.int/docs/default-source/coronaviruse/situation-reports/20200402-sitrep-73-covid-19.pdf?sfvrsn=5ae25bc7_2</t>
+  </si>
+  <si>
+    <t>Asymptomatic rate</t>
+  </si>
+  <si>
+    <t>https://www.eurosurveillance.org/content/10.2807/1560-7917.ES.2020.25.10.2000180</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov/coronavirus/2019-ncov/covid-data/covidview.html</t>
+  </si>
+  <si>
+    <t>Hospitalization rate</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Severe</t>
+  </si>
+  <si>
+    <t>Mild</t>
+  </si>
+  <si>
+    <t>Captured Cases</t>
+  </si>
+  <si>
+    <t>Total Cases</t>
+  </si>
+  <si>
+    <t>True Asymptomatic</t>
+  </si>
+  <si>
+    <t>Identifiable Cases</t>
+  </si>
+  <si>
+    <t>a + b + c + d = t</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>0.179t</t>
+  </si>
+  <si>
+    <t>d/t</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>a + b + c + 0.179t = t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a + b + c = </t>
+  </si>
+  <si>
+    <t>.82t</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>0.06c + 0.17c + c = 0.82t</t>
+  </si>
+  <si>
+    <t>0.06c + 0.17c + c + 0.179t = t</t>
+  </si>
+  <si>
+    <t>1.23c + 0.179t = t</t>
+  </si>
+  <si>
+    <t>1.23c = 0.82t</t>
+  </si>
+  <si>
+    <t>1.5c = t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">319 / 13438 </t>
+  </si>
+  <si>
+    <t>Case growth rate</t>
+  </si>
+  <si>
+    <t>Cases captured by type of case</t>
+  </si>
+  <si>
+    <t>https://www.baldingsworld.com/2020/03/29/how-fast-is-corona-spreading-and-how-many-undetected-cases-are-there/?fbclid=IwAR3eIpnPl4VhV3ypLNHVKdM002fz27uq1wz27gMeU7qgY3a2_eT3QOQutPw</t>
+  </si>
+  <si>
+    <t>https://www.nationalreview.com/2020/03/coronavirus-fatality-rate-computing-difficult/#slide-1</t>
+  </si>
+  <si>
+    <t>https://www.nationalreview.com/2020/03/coronavirus-pandemic-doctors-take-serious-disease-shutdown-approach-may-be-imperfect/#slide-1</t>
+  </si>
 </sst>
 </file>
 
@@ -424,7 +536,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,6 +598,25 @@
       <color rgb="FF2E2E2E"/>
       <name val="Georgia"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FFE6E1DC"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FFFC6F09"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="13"/>
+      <color rgb="FFE6E1DC"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -600,7 +731,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -669,6 +800,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1063,6 +1206,67 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>524752</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>285086</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="Severity of coronavirus cases in china 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A259696-ED2F-475A-A943-94A2610F42D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="20349882" y="1770529"/>
+          <a:ext cx="2945223" cy="2638322"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1329,100 +1533,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:R44"/>
+  <dimension ref="D1:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D7" s="1" t="s">
+    <row r="9" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D8" s="1" t="s">
+    <row r="10" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D9" s="1" t="s">
+    <row r="11" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D11" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D19" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
         <v>81</v>
       </c>
@@ -1436,7 +1650,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D23" s="1" t="s">
         <v>82</v>
       </c>
@@ -1451,17 +1665,17 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="24" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D24" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D25" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D26" s="1" t="s">
         <v>87</v>
       </c>
@@ -1469,7 +1683,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="s">
         <v>103</v>
       </c>
@@ -1485,7 +1699,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:18" x14ac:dyDescent="0.25">
       <c r="N28">
         <f>AVERAGE(810, 140)</f>
         <v>475</v>
@@ -1495,7 +1709,7 @@
         <v>1.7495395948434623E-2</v>
       </c>
     </row>
-    <row r="29" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D29" s="1" t="s">
         <v>112</v>
       </c>
@@ -1504,65 +1718,65 @@
         <v>27150</v>
       </c>
     </row>
-    <row r="30" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D30" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D31" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="4:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D32" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="4:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="18"/>
     </row>
-    <row r="41" spans="4:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="19" t="s">
         <v>92</v>
       </c>
@@ -1570,12 +1784,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D16" r:id="rId1" location="S2" display="S2" xr:uid="{E016D803-36A3-45D0-BE0C-0CF81E372776}"/>
-    <hyperlink ref="D6" r:id="rId2" location="bib0025" display="bib0025" xr:uid="{2A3FF179-05E8-4DE0-A18D-A77933B2B3F8}"/>
-    <hyperlink ref="D7" r:id="rId3" xr:uid="{3D709EE6-5160-4030-93B9-3969A9356103}"/>
-    <hyperlink ref="D8" r:id="rId4" xr:uid="{616ED8E6-40D1-4D61-9E14-CF2D2760AFB7}"/>
+    <hyperlink ref="D8" r:id="rId2" location="bib0025" display="bib0025" xr:uid="{2A3FF179-05E8-4DE0-A18D-A77933B2B3F8}"/>
+    <hyperlink ref="D9" r:id="rId3" xr:uid="{3D709EE6-5160-4030-93B9-3969A9356103}"/>
+    <hyperlink ref="D10" r:id="rId4" xr:uid="{616ED8E6-40D1-4D61-9E14-CF2D2760AFB7}"/>
     <hyperlink ref="D3" r:id="rId5" xr:uid="{A0C9FDAD-377D-41BD-9752-D6043B6B426E}"/>
     <hyperlink ref="D2" r:id="rId6" xr:uid="{760C8F73-DAD9-44A1-8506-3FDE74F815F5}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{95D651F1-B392-47F1-8B3A-08AE76E84FCA}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{95D651F1-B392-47F1-8B3A-08AE76E84FCA}"/>
     <hyperlink ref="D12" r:id="rId8" xr:uid="{DE4BBBB1-FDF0-4AE5-8147-C20927CDFC67}"/>
     <hyperlink ref="D15" r:id="rId9" xr:uid="{B25FF967-44D3-432C-8777-40DA96F17A7E}"/>
     <hyperlink ref="D14" r:id="rId10" xr:uid="{7C986D2A-E873-4721-9A3F-F9EEEECCD247}"/>
@@ -1599,29 +1813,360 @@
     <hyperlink ref="D34" r:id="rId28" xr:uid="{BC2124EB-8AF7-4071-B66B-C863476AD2EA}"/>
     <hyperlink ref="D35" r:id="rId29" xr:uid="{0F82DACF-9546-4BFE-BA6C-391D28757EF3}"/>
     <hyperlink ref="D29" r:id="rId30" xr:uid="{C7889458-3269-414C-9333-27436CF7008C}"/>
-    <hyperlink ref="D11" r:id="rId31" xr:uid="{F68D2B68-E29A-4C59-AA25-381D80FDD725}"/>
+    <hyperlink ref="D1" r:id="rId31" xr:uid="{EA1CEE00-04A5-4E81-AB41-BADD29285011}"/>
+    <hyperlink ref="D5" r:id="rId32" location="slide-1" display="https://www.nationalreview.com/2020/03/coronavirus-fatality-rate-computing-difficult/ - slide-1" xr:uid="{CBFCF224-F92B-4F6B-8C80-8AC21BA45F5F}"/>
+    <hyperlink ref="D6" r:id="rId33" location="slide-1" display="https://www.nationalreview.com/2020/03/coronavirus-pandemic-doctors-take-serious-disease-shutdown-approach-may-be-imperfect/ - slide-1" xr:uid="{6ABFA900-3386-40FD-B0E9-1D23EB79F04D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
-  <drawing r:id="rId33"/>
+  <pageSetup orientation="portrait" r:id="rId34"/>
+  <drawing r:id="rId35"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7BD97A-1146-4228-8E8F-D571B171B813}">
+  <dimension ref="C4:P45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>128</v>
+      </c>
+      <c r="J23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="29">
+        <v>0.05</v>
+      </c>
+      <c r="G24">
+        <f>F24*100</f>
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <f>G24/$G$31</f>
+        <v>4.1049999999999996E-2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>137</v>
+      </c>
+      <c r="J24" s="22">
+        <f>F24/$F$26</f>
+        <v>6.1728395061728392E-2</v>
+      </c>
+      <c r="K24">
+        <f>J24/$G$44</f>
+        <v>4.1049999999999996E-2</v>
+      </c>
+      <c r="L24">
+        <f>SUM(K24:K25)</f>
+        <v>0.15599000000000002</v>
+      </c>
+      <c r="M24">
+        <v>0.9</v>
+      </c>
+      <c r="N24">
+        <f>M24*L24</f>
+        <v>0.14039100000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="29">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G25">
+        <f>F25*100</f>
+        <v>14.000000000000002</v>
+      </c>
+      <c r="H25">
+        <f>G25/$G$31</f>
+        <v>0.11494000000000001</v>
+      </c>
+      <c r="I25" t="s">
+        <v>138</v>
+      </c>
+      <c r="J25" s="22">
+        <f>F25/$F$26</f>
+        <v>0.17283950617283952</v>
+      </c>
+      <c r="K25">
+        <f>J25/$G$44</f>
+        <v>0.11494000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" s="29">
+        <f>1-SUM(F24:F25)</f>
+        <v>0.81</v>
+      </c>
+      <c r="G26">
+        <f>F26*100</f>
+        <v>81</v>
+      </c>
+      <c r="H26">
+        <f>G26/$G$31</f>
+        <v>0.66500999999999999</v>
+      </c>
+      <c r="I26" t="s">
+        <v>130</v>
+      </c>
+      <c r="J26" s="22">
+        <f>F26/$F$26</f>
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <f>J26/$G$44</f>
+        <v>0.66500999999999999</v>
+      </c>
+      <c r="M26">
+        <v>0.25</v>
+      </c>
+      <c r="N26">
+        <f>M26*K26</f>
+        <v>0.1662525</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="J27" s="31">
+        <f>SUM(J24:J26)</f>
+        <v>1.2345679012345678</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="30">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="G28">
+        <f>F28*100</f>
+        <v>17.899999999999999</v>
+      </c>
+      <c r="H28">
+        <f>G28/$G$31</f>
+        <v>0.14695899999999998</v>
+      </c>
+      <c r="K28">
+        <f>1-SUM(K24:K26)</f>
+        <v>0.17900000000000005</v>
+      </c>
+      <c r="M28">
+        <v>0.01</v>
+      </c>
+      <c r="N28">
+        <f>M28*K28</f>
+        <v>1.7900000000000006E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30">
+        <f>SUM(G24:G26)</f>
+        <v>100</v>
+      </c>
+      <c r="N30">
+        <f>SUM(N24:N28)</f>
+        <v>0.30843350000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>126</v>
+      </c>
+      <c r="G31">
+        <f>G30/(1-F28)</f>
+        <v>121.8026796589525</v>
+      </c>
+    </row>
+    <row r="33" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>132</v>
+      </c>
+      <c r="H34">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="P34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="7:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H35" t="s">
+        <v>131</v>
+      </c>
+      <c r="L35" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="P35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="7:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L36" s="33">
+        <v>13438</v>
+      </c>
+      <c r="M36">
+        <f>L36/N30</f>
+        <v>43568.548811980538</v>
+      </c>
+    </row>
+    <row r="37" spans="7:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>134</v>
+      </c>
+      <c r="L37" s="34">
+        <v>319</v>
+      </c>
+      <c r="M37">
+        <f>L37/0.9</f>
+        <v>354.44444444444446</v>
+      </c>
+      <c r="N37">
+        <f>M37/M36</f>
+        <v>8.1353282151775241E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>135</v>
+      </c>
+      <c r="H39" s="30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G44" s="31">
+        <f>J27/(1-F28)</f>
+        <v>1.5037367859129938</v>
+      </c>
+    </row>
+    <row r="45" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{356FED09-864D-42B1-9734-3ABB7F56A365}"/>
+    <hyperlink ref="C9" r:id="rId2" xr:uid="{F68D2B68-E29A-4C59-AA25-381D80FDD725}"/>
+    <hyperlink ref="C14" r:id="rId3" xr:uid="{B64D5734-DC18-4493-B22C-A40B22A6340E}"/>
+    <hyperlink ref="C15" r:id="rId4" xr:uid="{90A38EB1-7C22-479C-91C6-6193068E6AE9}"/>
+    <hyperlink ref="C20" r:id="rId5" xr:uid="{CAE48047-1268-4B85-80EC-C8C071A160B3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F961DF-88C5-4FC4-A498-BDBE2D214606}">
   <dimension ref="C3:Q44"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="12.109375" customWidth="1"/>
-    <col min="17" max="17" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>72</v>
       </c>
@@ -1630,7 +2175,7 @@
         <v>1.4732E-3</v>
       </c>
     </row>
-    <row r="4" spans="3:16" ht="61.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:16" ht="78.75" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1661,7 +2206,7 @@
       </c>
       <c r="O4" s="28"/>
     </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1696,7 +2241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1731,7 +2276,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:16" ht="56.25" x14ac:dyDescent="0.25">
       <c r="C7" s="23" t="s">
         <v>18</v>
       </c>
@@ -1776,7 +2321,7 @@
         <v>6.5010000000000003E-4</v>
       </c>
     </row>
-    <row r="8" spans="3:16" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:16" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="24"/>
       <c r="D8" s="8" t="s">
         <v>21</v>
@@ -1814,7 +2359,7 @@
       </c>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="3:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:16" ht="45" x14ac:dyDescent="0.25">
       <c r="C9" s="23" t="s">
         <v>32</v>
       </c>
@@ -1859,7 +2404,7 @@
         <v>1.4732E-3</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:16" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="24"/>
       <c r="D10" s="8" t="s">
         <v>36</v>
@@ -1897,7 +2442,7 @@
       </c>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" spans="3:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:16" ht="56.25" x14ac:dyDescent="0.25">
       <c r="C11" s="23" t="s">
         <v>47</v>
       </c>
@@ -1942,7 +2487,7 @@
         <v>7.6810000000000008E-4</v>
       </c>
     </row>
-    <row r="12" spans="3:16" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:16" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="24"/>
       <c r="D12" s="8" t="s">
         <v>49</v>
@@ -1980,7 +2525,7 @@
       </c>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="3:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:16" ht="56.25" x14ac:dyDescent="0.25">
       <c r="C13" s="23" t="s">
         <v>59</v>
       </c>
@@ -2025,7 +2570,7 @@
         <v>1.4343000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="3:16" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:16" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="24"/>
       <c r="D14" s="8" t="s">
         <v>62</v>
@@ -2062,7 +2607,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H35" s="21" t="s">
         <v>99</v>
       </c>
@@ -2100,7 +2645,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
         <v>97</v>
       </c>
@@ -2133,7 +2678,7 @@
         <v>3.7874999999999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H37" t="s">
         <v>96</v>
       </c>
@@ -2166,7 +2711,7 @@
         <v>0.44087499999999996</v>
       </c>
     </row>
-    <row r="38" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H38" t="s">
         <v>95</v>
       </c>
@@ -2199,7 +2744,7 @@
         <v>27.787500000000001</v>
       </c>
     </row>
-    <row r="40" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H40" t="s">
         <v>94</v>
       </c>
@@ -2240,7 +2785,7 @@
         <v>1.5865946918578497E-2</v>
       </c>
     </row>
-    <row r="42" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H42" t="s">
         <v>98</v>
       </c>
@@ -2248,7 +2793,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="44" spans="8:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="8:17" x14ac:dyDescent="0.25">
       <c r="H44" t="s">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
cleaning up code, adding new R0 calculations, new state map, test rates vs case fatality rates
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
+++ b/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy\Projects\COVID-19\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BB7576-74FE-4EC2-9565-008FD3DD90B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A0EE68-2A5C-4DA4-89FB-B5A56A68E7E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2385" yWindow="3975" windowWidth="20550" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="153">
   <si>
     <t>https://www.cdc.gov/flu/weekly/#S2</t>
   </si>
@@ -526,6 +526,12 @@
   </si>
   <si>
     <t>https://www.nationalreview.com/2020/03/coronavirus-pandemic-doctors-take-serious-disease-shutdown-approach-may-be-imperfect/#slide-1</t>
+  </si>
+  <si>
+    <t>https://www.vox.com/future-perfect/2020/3/12/21172040/coronavirus-covid-19-virus-charts</t>
+  </si>
+  <si>
+    <t>https://www.nationalreview.com/2020/04/coronavirus-response-sweden-avoids-isolation-economic-ruin/</t>
   </si>
 </sst>
 </file>
@@ -783,6 +789,18 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -800,18 +818,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1533,10 +1539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D1:R44"/>
+  <dimension ref="D1:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,6 +1602,11 @@
         <v>73</v>
       </c>
     </row>
+    <row r="13" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
     <row r="14" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>75</v>
@@ -1779,6 +1790,11 @@
     <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="19" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1816,10 +1832,12 @@
     <hyperlink ref="D1" r:id="rId31" xr:uid="{EA1CEE00-04A5-4E81-AB41-BADD29285011}"/>
     <hyperlink ref="D5" r:id="rId32" location="slide-1" display="https://www.nationalreview.com/2020/03/coronavirus-fatality-rate-computing-difficult/ - slide-1" xr:uid="{CBFCF224-F92B-4F6B-8C80-8AC21BA45F5F}"/>
     <hyperlink ref="D6" r:id="rId33" location="slide-1" display="https://www.nationalreview.com/2020/03/coronavirus-pandemic-doctors-take-serious-disease-shutdown-approach-may-be-imperfect/ - slide-1" xr:uid="{6ABFA900-3386-40FD-B0E9-1D23EB79F04D}"/>
+    <hyperlink ref="D13" r:id="rId34" xr:uid="{CE42E117-3951-4B6A-94C5-EABEF166E558}"/>
+    <hyperlink ref="D47" r:id="rId35" xr:uid="{4B8B5855-4E3A-4763-B56D-5BF111E1980F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
-  <drawing r:id="rId35"/>
+  <pageSetup orientation="portrait" r:id="rId36"/>
+  <drawing r:id="rId37"/>
 </worksheet>
 </file>
 
@@ -1894,7 +1912,7 @@
       <c r="E24" t="s">
         <v>122</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F24" s="23">
         <v>0.05</v>
       </c>
       <c r="G24">
@@ -1932,7 +1950,7 @@
       <c r="E25" t="s">
         <v>123</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F25" s="23">
         <v>0.14000000000000001</v>
       </c>
       <c r="G25">
@@ -1959,7 +1977,7 @@
       <c r="E26" t="s">
         <v>124</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="23">
         <f>1-SUM(F24:F25)</f>
         <v>0.81</v>
       </c>
@@ -1991,7 +2009,7 @@
       </c>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="J27" s="31">
+      <c r="J27" s="25">
         <f>SUM(J24:J26)</f>
         <v>1.2345679012345678</v>
       </c>
@@ -2000,7 +2018,7 @@
       <c r="E28" t="s">
         <v>127</v>
       </c>
-      <c r="F28" s="30">
+      <c r="F28" s="24">
         <v>0.17899999999999999</v>
       </c>
       <c r="G28">
@@ -2068,7 +2086,7 @@
       <c r="H35" t="s">
         <v>131</v>
       </c>
-      <c r="L35" s="32" t="s">
+      <c r="L35" s="26" t="s">
         <v>145</v>
       </c>
       <c r="P35" t="s">
@@ -2076,7 +2094,7 @@
       </c>
     </row>
     <row r="36" spans="7:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="L36" s="33">
+      <c r="L36" s="27">
         <v>13438</v>
       </c>
       <c r="M36">
@@ -2088,7 +2106,7 @@
       <c r="G37" t="s">
         <v>134</v>
       </c>
-      <c r="L37" s="34">
+      <c r="L37" s="28">
         <v>319</v>
       </c>
       <c r="M37">
@@ -2104,7 +2122,7 @@
       <c r="G39" t="s">
         <v>135</v>
       </c>
-      <c r="H39" s="30" t="s">
+      <c r="H39" s="24" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2129,7 +2147,7 @@
       </c>
     </row>
     <row r="44" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G44" s="31">
+      <c r="G44" s="25">
         <f>J27/(1-F28)</f>
         <v>1.5037367859129938</v>
       </c>
@@ -2185,26 +2203,26 @@
       <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="27" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="27" t="s">
+      <c r="I4" s="34"/>
+      <c r="J4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="27" t="s">
+      <c r="K4" s="34"/>
+      <c r="L4" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="28"/>
-      <c r="N4" s="27" t="s">
+      <c r="M4" s="34"/>
+      <c r="N4" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="28"/>
+      <c r="O4" s="34"/>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
@@ -2277,13 +2295,13 @@
       </c>
     </row>
     <row r="7" spans="3:16" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="29" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="12">
@@ -2322,11 +2340,11 @@
       </c>
     </row>
     <row r="8" spans="3:16" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="24"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="26"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="13" t="s">
         <v>22</v>
       </c>
@@ -2360,13 +2378,13 @@
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="3:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="29" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="31" t="s">
         <v>34</v>
       </c>
       <c r="F9" s="12">
@@ -2405,11 +2423,11 @@
       </c>
     </row>
     <row r="10" spans="3:16" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="24"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="26"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="13" t="s">
         <v>37</v>
       </c>
@@ -2443,13 +2461,13 @@
       <c r="P10" s="4"/>
     </row>
     <row r="11" spans="3:16" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="29" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="31" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="12">
@@ -2488,11 +2506,11 @@
       </c>
     </row>
     <row r="12" spans="3:16" ht="57" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="24"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="26"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="13" t="s">
         <v>50</v>
       </c>
@@ -2526,13 +2544,13 @@
       <c r="P12" s="4"/>
     </row>
     <row r="13" spans="3:16" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="29" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="31" t="s">
         <v>61</v>
       </c>
       <c r="F13" s="12">
@@ -2571,11 +2589,11 @@
       </c>
     </row>
     <row r="14" spans="3:16" ht="57" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="24"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="26"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="13" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
initial work on infection mortality rates in Italy, adding imhe data
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
+++ b/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy\Projects\COVID-19\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A0EE68-2A5C-4DA4-89FB-B5A56A68E7E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B671D9B-73B5-416E-BF0A-27A1241B1B21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="3975" windowWidth="20550" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1644" yWindow="2604" windowWidth="16440" windowHeight="7992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="160">
   <si>
     <t>https://www.cdc.gov/flu/weekly/#S2</t>
   </si>
@@ -532,6 +532,27 @@
   </si>
   <si>
     <t>https://www.nationalreview.com/2020/04/coronavirus-response-sweden-avoids-isolation-economic-ruin/</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/2003.00122.pdf</t>
+  </si>
+  <si>
+    <t>https://www.reuters.com/article/us-health-coronavirus-britain-spread/preliminary-study-finds-uk-lockdown-is-slowing-spread-of-covid-19-idUSKBN21J56W</t>
+  </si>
+  <si>
+    <t>lockdown - social distancing effects -- 70% r0 reduction</t>
+  </si>
+  <si>
+    <t>https://www.medrxiv.org/content/10.1101/2020.04.02.20051466v1.full.pdf</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pubmed/32202261</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/2020/04/05/us/coronavirus-deaths-undercount.html?referringSource=articleShare</t>
+  </si>
+  <si>
+    <t>https://reason.com/2020/04/09/preliminary-german-study-shows-a-covid-19-infection-fatality-rate-of-about-0-4-percent/</t>
   </si>
 </sst>
 </file>
@@ -1539,115 +1560,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D1:R47"/>
+  <dimension ref="D1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D12" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D13" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D14" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D15" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D17" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D18" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D19" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D20" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D21" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D22" s="1" t="s">
         <v>81</v>
       </c>
@@ -1661,7 +1682,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D23" s="1" t="s">
         <v>82</v>
       </c>
@@ -1676,17 +1697,17 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="24" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D24" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D25" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D26" s="1" t="s">
         <v>87</v>
       </c>
@@ -1694,7 +1715,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D27" s="1" t="s">
         <v>103</v>
       </c>
@@ -1710,7 +1731,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:18" x14ac:dyDescent="0.3">
       <c r="N28">
         <f>AVERAGE(810, 140)</f>
         <v>475</v>
@@ -1720,7 +1741,7 @@
         <v>1.7495395948434623E-2</v>
       </c>
     </row>
-    <row r="29" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D29" s="1" t="s">
         <v>112</v>
       </c>
@@ -1729,72 +1750,110 @@
         <v>27150</v>
       </c>
     </row>
-    <row r="30" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D30" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D31" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D32" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4" ht="15" x14ac:dyDescent="0.3">
       <c r="D38" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40" s="18"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4" ht="15" x14ac:dyDescent="0.3">
       <c r="D41" s="16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D44" s="19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D47" s="1" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D51" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D52" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D54" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D57" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1834,10 +1893,15 @@
     <hyperlink ref="D6" r:id="rId33" location="slide-1" display="https://www.nationalreview.com/2020/03/coronavirus-pandemic-doctors-take-serious-disease-shutdown-approach-may-be-imperfect/ - slide-1" xr:uid="{6ABFA900-3386-40FD-B0E9-1D23EB79F04D}"/>
     <hyperlink ref="D13" r:id="rId34" xr:uid="{CE42E117-3951-4B6A-94C5-EABEF166E558}"/>
     <hyperlink ref="D47" r:id="rId35" xr:uid="{4B8B5855-4E3A-4763-B56D-5BF111E1980F}"/>
+    <hyperlink ref="D49" r:id="rId36" xr:uid="{657340A7-A2E6-444B-80F7-4164B6B388FD}"/>
+    <hyperlink ref="D51" r:id="rId37" xr:uid="{217EA91C-9C49-4581-B2A0-7FE83E2B093E}"/>
+    <hyperlink ref="D54" r:id="rId38" xr:uid="{ACE5A0B8-594A-494E-B6DD-C42E9F9354E5}"/>
+    <hyperlink ref="D52" r:id="rId39" xr:uid="{ADD8846A-EA2C-4430-A0D9-412279CEB920}"/>
+    <hyperlink ref="D57" r:id="rId40" xr:uid="{486FFE65-AD09-4040-8256-29091780E43D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
-  <drawing r:id="rId37"/>
+  <pageSetup orientation="portrait" r:id="rId41"/>
+  <drawing r:id="rId42"/>
 </worksheet>
 </file>
 
@@ -1849,58 +1913,58 @@
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>128</v>
       </c>
@@ -1908,7 +1972,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>122</v>
       </c>
@@ -1946,7 +2010,7 @@
         <v>0.14039100000000002</v>
       </c>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>123</v>
       </c>
@@ -1973,7 +2037,7 @@
         <v>0.11494000000000001</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>124</v>
       </c>
@@ -2008,13 +2072,13 @@
         <v>0.1662525</v>
       </c>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
       <c r="J27" s="25">
         <f>SUM(J24:J26)</f>
         <v>1.2345679012345678</v>
       </c>
     </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>127</v>
       </c>
@@ -2041,7 +2105,7 @@
         <v>1.7900000000000006E-3</v>
       </c>
     </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
         <v>125</v>
       </c>
@@ -2054,7 +2118,7 @@
         <v>0.30843350000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:14" x14ac:dyDescent="0.3">
       <c r="E31" t="s">
         <v>126</v>
       </c>
@@ -2063,12 +2127,12 @@
         <v>121.8026796589525</v>
       </c>
     </row>
-    <row r="33" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G33" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G34" t="s">
         <v>132</v>
       </c>
@@ -2079,7 +2143,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="7:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:16" ht="16.8" x14ac:dyDescent="0.3">
       <c r="G35" t="s">
         <v>133</v>
       </c>
@@ -2093,7 +2157,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="7:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:16" ht="16.8" x14ac:dyDescent="0.3">
       <c r="L36" s="27">
         <v>13438</v>
       </c>
@@ -2102,7 +2166,7 @@
         <v>43568.548811980538</v>
       </c>
     </row>
-    <row r="37" spans="7:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:16" ht="16.8" x14ac:dyDescent="0.3">
       <c r="G37" t="s">
         <v>134</v>
       </c>
@@ -2118,7 +2182,7 @@
         <v>8.1353282151775241E-3</v>
       </c>
     </row>
-    <row r="39" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G39" t="s">
         <v>135</v>
       </c>
@@ -2126,33 +2190,33 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G40" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G41" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G42" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G43" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G44" s="25">
         <f>J27/(1-F28)</f>
         <v>1.5037367859129938</v>
       </c>
     </row>
-    <row r="45" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G45" t="s">
         <v>144</v>
       </c>
@@ -2178,13 +2242,13 @@
       <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>72</v>
       </c>
@@ -2193,7 +2257,7 @@
         <v>1.4732E-3</v>
       </c>
     </row>
-    <row r="4" spans="3:16" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:16" ht="61.2" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
@@ -2224,7 +2288,7 @@
       </c>
       <c r="O4" s="34"/>
     </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2259,7 +2323,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -2294,7 +2358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="C7" s="29" t="s">
         <v>18</v>
       </c>
@@ -2339,7 +2403,7 @@
         <v>6.5010000000000003E-4</v>
       </c>
     </row>
-    <row r="8" spans="3:16" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:16" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="30"/>
       <c r="D8" s="8" t="s">
         <v>21</v>
@@ -2377,7 +2441,7 @@
       </c>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="3:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="C9" s="29" t="s">
         <v>32</v>
       </c>
@@ -2422,7 +2486,7 @@
         <v>1.4732E-3</v>
       </c>
     </row>
-    <row r="10" spans="3:16" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:16" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="30"/>
       <c r="D10" s="8" t="s">
         <v>36</v>
@@ -2460,7 +2524,7 @@
       </c>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" spans="3:16" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="C11" s="29" t="s">
         <v>47</v>
       </c>
@@ -2505,7 +2569,7 @@
         <v>7.6810000000000008E-4</v>
       </c>
     </row>
-    <row r="12" spans="3:16" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:16" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="30"/>
       <c r="D12" s="8" t="s">
         <v>49</v>
@@ -2543,7 +2607,7 @@
       </c>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="3:16" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:16" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="C13" s="29" t="s">
         <v>59</v>
       </c>
@@ -2588,7 +2652,7 @@
         <v>1.4343000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="3:16" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:16" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="30"/>
       <c r="D14" s="8" t="s">
         <v>62</v>
@@ -2625,7 +2689,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H35" s="21" t="s">
         <v>99</v>
       </c>
@@ -2663,7 +2727,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H36" t="s">
         <v>97</v>
       </c>
@@ -2696,7 +2760,7 @@
         <v>3.7874999999999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H37" t="s">
         <v>96</v>
       </c>
@@ -2729,7 +2793,7 @@
         <v>0.44087499999999996</v>
       </c>
     </row>
-    <row r="38" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H38" t="s">
         <v>95</v>
       </c>
@@ -2762,7 +2826,7 @@
         <v>27.787500000000001</v>
       </c>
     </row>
-    <row r="40" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H40" t="s">
         <v>94</v>
       </c>
@@ -2803,7 +2867,7 @@
         <v>1.5865946918578497E-2</v>
       </c>
     </row>
-    <row r="42" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H42" t="s">
         <v>98</v>
       </c>
@@ -2811,7 +2875,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="44" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H44" t="s">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
daily plot update, work on extracting Italian flu deaths by season
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
+++ b/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy\Projects\COVID-19\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B671D9B-73B5-416E-BF0A-27A1241B1B21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844ECCF7-42C6-406D-94BC-5D2B4B0DDA64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1644" yWindow="2604" windowWidth="16440" windowHeight="7992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="162">
   <si>
     <t>https://www.cdc.gov/flu/weekly/#S2</t>
   </si>
@@ -553,6 +553,12 @@
   </si>
   <si>
     <t>https://reason.com/2020/04/09/preliminary-german-study-shows-a-covid-19-infection-fatality-rate-of-about-0-4-percent/</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/d41586-020-00885-w</t>
+  </si>
+  <si>
+    <t>https://www.medrxiv.org/content/10.1101/2020.03.05.20031773v2</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -1909,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7BD97A-1146-4228-8E8F-D571B171B813}">
   <dimension ref="C4:P45"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1939,6 +1945,16 @@
         <v>113</v>
       </c>
     </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
     <row r="13" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>118</v>
@@ -1952,6 +1968,11 @@
     <row r="15" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.3">
@@ -2228,9 +2249,12 @@
     <hyperlink ref="C14" r:id="rId3" xr:uid="{B64D5734-DC18-4493-B22C-A40B22A6340E}"/>
     <hyperlink ref="C15" r:id="rId4" xr:uid="{90A38EB1-7C22-479C-91C6-6193068E6AE9}"/>
     <hyperlink ref="C20" r:id="rId5" xr:uid="{CAE48047-1268-4B85-80EC-C8C071A160B3}"/>
+    <hyperlink ref="C10" r:id="rId6" xr:uid="{94788B57-BDBA-4EDF-8039-264B0B5D2867}"/>
+    <hyperlink ref="C16" r:id="rId7" xr:uid="{1CF4BB12-397A-4D72-AAC6-5FBB38B055C2}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{39D77077-72AD-4727-993B-5E67EA9A33A9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
adding mobility index for all countries
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
+++ b/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy\Projects\COVID-19\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844ECCF7-42C6-406D-94BC-5D2B4B0DDA64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6F9B92-0F43-4D7C-B898-30601B0DAC06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature" sheetId="1" r:id="rId1"/>
     <sheet name="data sources" sheetId="3" r:id="rId2"/>
-    <sheet name="notes" sheetId="2" r:id="rId3"/>
+    <sheet name="response stringency" sheetId="4" r:id="rId3"/>
+    <sheet name="notes" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="165">
   <si>
     <t>https://www.cdc.gov/flu/weekly/#S2</t>
   </si>
@@ -559,6 +560,15 @@
   </si>
   <si>
     <t>https://www.medrxiv.org/content/10.1101/2020.03.05.20031773v2</t>
+  </si>
+  <si>
+    <t>https://www.cnn.com/2020/04/16/world/coronavirus-response-lessons-learned-intl/index.html?fbclid=IwAR0k7CpS5_FLMyJAFs3wyKrtJN5ds89hbYHtmYaa2CHJMliJ4GeEKz8IXeA</t>
+  </si>
+  <si>
+    <t>https://www.bsg.ox.ac.uk/research/research-projects/coronavirus-government-response-tracker</t>
+  </si>
+  <si>
+    <t>https://www.economist.com/graphic-detail/2020/04/13/deaths-from-cardiac-arrests-have-surged-in-new-york-city</t>
   </si>
 </sst>
 </file>
@@ -1915,7 +1925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7BD97A-1146-4228-8E8F-D571B171B813}">
   <dimension ref="C4:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -2259,6 +2269,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8208EEC2-AF54-496E-9035-B9168EA61C66}">
+  <dimension ref="C4:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{789BD8E9-0AE7-4C41-BDEB-145997D47DD7}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{B318EF3E-479F-44C6-B0E5-BF1F0268C60B}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{02DCEA97-385D-43B1-A52B-B8AD0DC69CF9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F961DF-88C5-4FC4-A498-BDBE2D214606}">
   <dimension ref="C3:Q44"/>
   <sheetViews>

</xml_diff>

<commit_message>
data update and sample simulation script
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
+++ b/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy\Projects\COVID-19\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9D1407-59E6-4648-8729-909F55B440D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7015656C-66B2-4917-A907-119D9E68744E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="174">
   <si>
     <t>https://www.cdc.gov/flu/weekly/#S2</t>
   </si>
@@ -581,6 +581,21 @@
   </si>
   <si>
     <t>https://www.nbcnewyork.com/news/local/new-york-virus-deaths-top-15k-cuomo-expected-to-detail-plan-to-fight-nursing-home-outbreaks/2386556/</t>
+  </si>
+  <si>
+    <t>https://www.wsj.com/articles/new-data-suggest-the-coronavirus-isnt-as-deadly-as-we-thought-11587155298</t>
+  </si>
+  <si>
+    <t>https://www.theguardian.com/world/2020/apr/23/coronavirus-antibody-studies-california-stanford</t>
+  </si>
+  <si>
+    <t>Immunity studies</t>
+  </si>
+  <si>
+    <t>https://www.washingtonpost.com/health/antibody-tests-support-whats-been-obvious-covid-19-is-much-more-lethal-than-flu/2020/04/28/2fc215d8-87f7-11ea-ac8a-fe9b8088e101_story.html</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/2020/04/28/opinion/coronavirus-testing.html</t>
   </si>
 </sst>
 </file>
@@ -1935,10 +1950,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7BD97A-1146-4228-8E8F-D571B171B813}">
-  <dimension ref="C4:P45"/>
+  <dimension ref="C2:P45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1947,52 +1962,75 @@
     <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="H4" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="H7" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
         <v>159</v>
       </c>
@@ -2274,9 +2312,13 @@
     <hyperlink ref="C10" r:id="rId6" xr:uid="{94788B57-BDBA-4EDF-8039-264B0B5D2867}"/>
     <hyperlink ref="C16" r:id="rId7" xr:uid="{1CF4BB12-397A-4D72-AAC6-5FBB38B055C2}"/>
     <hyperlink ref="C11" r:id="rId8" xr:uid="{39D77077-72AD-4727-993B-5E67EA9A33A9}"/>
+    <hyperlink ref="H3" r:id="rId9" xr:uid="{66F5974A-F5DA-4218-B540-72697765C5CE}"/>
+    <hyperlink ref="H4" r:id="rId10" xr:uid="{25680931-4B9D-42EF-96F6-7C8B740C0A4E}"/>
+    <hyperlink ref="H6" r:id="rId11" xr:uid="{5DC2D781-DE0F-48FB-9B69-C8E183F9D6D0}"/>
+    <hyperlink ref="H7" r:id="rId12" xr:uid="{C500B2DC-B096-4E86-9D21-2B274D9E8A92}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -2284,7 +2326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8208EEC2-AF54-496E-9035-B9168EA61C66}">
   <dimension ref="C4:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
data update, new analyses on mobility/stringency data
</commit_message>
<xml_diff>
--- a/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
+++ b/Projects/COVID-19/literature/Italy Influenza vs. COVID.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csq\Documents\Public_Policy\Projects\COVID-19\literature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Public_Policy\Projects\COVID-19\literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7015656C-66B2-4917-A907-119D9E68744E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDD6BB2-3473-4156-BF92-B1B75EF0643F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="176">
   <si>
     <t>https://www.cdc.gov/flu/weekly/#S2</t>
   </si>
@@ -596,6 +598,12 @@
   </si>
   <si>
     <t>https://www.nytimes.com/2020/04/28/opinion/coronavirus-testing.html</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov/nchs/nvss/vsrr/covid19/index.htm?fbclid=IwAR3NFNvdjpDVd6eGvtEBIf8uDkI1IlxnXAXa0iR5B6y9lbJhUsoSMUCe7wM</t>
+  </si>
+  <si>
+    <t>Excess deaths cdc</t>
   </si>
 </sst>
 </file>
@@ -1952,8 +1960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7BD97A-1146-4228-8E8F-D571B171B813}">
   <dimension ref="C2:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2043,6 +2051,16 @@
     <row r="20" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.3">
@@ -2316,9 +2334,10 @@
     <hyperlink ref="H4" r:id="rId10" xr:uid="{25680931-4B9D-42EF-96F6-7C8B740C0A4E}"/>
     <hyperlink ref="H6" r:id="rId11" xr:uid="{5DC2D781-DE0F-48FB-9B69-C8E183F9D6D0}"/>
     <hyperlink ref="H7" r:id="rId12" xr:uid="{C500B2DC-B096-4E86-9D21-2B274D9E8A92}"/>
+    <hyperlink ref="C22" r:id="rId13" xr:uid="{5A761D66-92C2-4B5C-8025-6DECA0ED2A5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>